<commit_message>
relative imports fix + tests folder
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -450,87 +450,87 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="C2" t="n">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="D2" t="n">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="E2" t="n">
-        <v>94</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="D3" t="n">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="E3" t="n">
-        <v>91</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="B4" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="D4" t="n">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="E4" t="n">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B5" t="n">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="C5" t="n">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="D5" t="n">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="E5" t="n">
-        <v>16</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B6" t="n">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C6" t="n">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D6" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E6" t="n">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>